<commit_message>
Mejoras en el servidor para obtener laggard animes
</commit_message>
<xml_diff>
--- a/temporadas cargadas.xlsx
+++ b/temporadas cargadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Desktop\Git Ra-code\MoshiApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31103709-2648-4AC7-867D-F26CA4808A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC080E-C48C-430E-96E7-F0C7AB13B21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="4230" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t>Año</t>
   </si>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +97,12 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -146,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -160,6 +166,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,191 +448,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:O20"/>
+  <dimension ref="B3:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" customWidth="1"/>
-    <col min="15" max="15" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="5" customWidth="1"/>
+    <col min="8" max="8" width="0.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="N4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="C5" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="M5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="N5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="M7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="M8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="N7" s="2" t="s">
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5">
+        <v>1592193600000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5">
+        <v>1584244800000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5">
+        <v>1576382400000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5">
+        <v>1568520000000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="N8" s="3" t="s">
+      <c r="D20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5">
+        <v>1560571200000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1552622400000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
-        <v>2022</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="G22" s="5">
+        <v>1544846400000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1536984000000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1529035200000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="4">
-        <v>2021</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="G25" s="5">
+        <v>1521086400000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G26" s="5">
+        <v>1513310400000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1505448000000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1497499200000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1489550400000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correccion error vencimiento token de video. Correccion no mostrar enimes sin episodios
</commit_message>
<xml_diff>
--- a/temporadas cargadas.xlsx
+++ b/temporadas cargadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Desktop\Git Ra-code\MoshiApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC080E-C48C-430E-96E7-F0C7AB13B21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1FF81F-23F5-45ED-BC55-95312870D9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4245" yWindow="4230" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>Año</t>
   </si>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,6 +618,9 @@
         <v>13</v>
       </c>
       <c r="F13" s="4"/>
+      <c r="G13" s="5">
+        <v>1615780800000</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
@@ -650,7 +653,9 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="5">
         <v>1592193600000</v>

</xml_diff>